<commit_message>
testing on final sets of images
</commit_message>
<xml_diff>
--- a/illumination/metrics.xlsx
+++ b/illumination/metrics.xlsx
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>